<commit_message>
Add references to requirements tracker
</commit_message>
<xml_diff>
--- a/test/_requirements/requirements_tracker.xlsx
+++ b/test/_requirements/requirements_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markchalinder/Documents/GitHub/Rails6/alpha-blog/test/_requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markchalinder/Documents/GitHub/Rails6/aws-eb-demo/test/_requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F74CE4A-1545-9F4A-9D9F-C08C6274862E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E5A8F6-C216-EC4E-A81F-B0EA4ECCB228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{74C67756-0067-1D4A-A044-D3ADD871B77F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>Implemented in</t>
   </si>
@@ -117,16 +117,130 @@
   </si>
   <si>
     <t>app/views/articles/show.html.erb</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>A.1</t>
+  </si>
+  <si>
+    <t>A.2</t>
+  </si>
+  <si>
+    <t>A.3</t>
+  </si>
+  <si>
+    <t>A.4</t>
+  </si>
+  <si>
+    <t>A.5</t>
+  </si>
+  <si>
+    <t>A.6</t>
+  </si>
+  <si>
+    <t>A.7</t>
+  </si>
+  <si>
+    <t>A.8</t>
+  </si>
+  <si>
+    <t>A.9</t>
+  </si>
+  <si>
+    <t>A.10</t>
+  </si>
+  <si>
+    <t>A.11</t>
+  </si>
+  <si>
+    <t>A.12</t>
+  </si>
+  <si>
+    <t>A.13</t>
+  </si>
+  <si>
+    <t>A.14</t>
+  </si>
+  <si>
+    <t>A.15</t>
+  </si>
+  <si>
+    <t>A.16</t>
+  </si>
+  <si>
+    <t>A.17</t>
+  </si>
+  <si>
+    <t>A.18</t>
+  </si>
+  <si>
+    <t>A.19</t>
+  </si>
+  <si>
+    <t>A.20</t>
+  </si>
+  <si>
+    <t>A.21</t>
+  </si>
+  <si>
+    <t>B.1</t>
+  </si>
+  <si>
+    <t>B.2</t>
+  </si>
+  <si>
+    <t>B.3</t>
+  </si>
+  <si>
+    <t>B.4</t>
+  </si>
+  <si>
+    <t>B.5</t>
+  </si>
+  <si>
+    <t>B.6</t>
+  </si>
+  <si>
+    <t>B.7</t>
+  </si>
+  <si>
+    <t>C.1</t>
+  </si>
+  <si>
+    <t>C.2</t>
+  </si>
+  <si>
+    <t>C.3</t>
+  </si>
+  <si>
+    <t>C.4</t>
+  </si>
+  <si>
+    <t>C.5</t>
+  </si>
+  <si>
+    <t>C.6</t>
+  </si>
+  <si>
+    <t>C.7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,9 +312,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -210,7 +325,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,239 +643,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9C0EC-30A0-144D-9AD5-FB8E9C5B121B}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B32" sqref="B32:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="118.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" customWidth="1"/>
+    <col min="1" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="118.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B24" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -765,6 +1004,7 @@
     <mergeCell ref="A2:A22"/>
     <mergeCell ref="A32:A38"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add conditional around gem tzinfo-data in Gemfile
</commit_message>
<xml_diff>
--- a/test/_requirements/requirements_tracker.xlsx
+++ b/test/_requirements/requirements_tracker.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markchalinder/Documents/GitHub/Rails6/aws-eb-demo/test/_requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFC8DD2-50E0-3647-8F9F-2B6686EF642E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E74182F-C3CB-A148-B4BB-B860EBDBA531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33480" windowHeight="18480" xr2:uid="{74C67756-0067-1D4A-A044-D3ADD871B77F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33480" windowHeight="18480" activeTab="1" xr2:uid="{74C67756-0067-1D4A-A044-D3ADD871B77F}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="BUGS &amp; Issues" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>Implemented in</t>
   </si>
@@ -256,6 +256,69 @@
   </si>
   <si>
     <t>Use .ebextensions to create Redis ElastiCache</t>
+  </si>
+  <si>
+    <t>ISS.001</t>
+  </si>
+  <si>
+    <t>ISS.002</t>
+  </si>
+  <si>
+    <t>ISS.003</t>
+  </si>
+  <si>
+    <t>ISS.004</t>
+  </si>
+  <si>
+    <t>ISS.005</t>
+  </si>
+  <si>
+    <t>ISS.006</t>
+  </si>
+  <si>
+    <t>ISS.007</t>
+  </si>
+  <si>
+    <t>ISS.008</t>
+  </si>
+  <si>
+    <t>ISS.009</t>
+  </si>
+  <si>
+    <t>ISS.010</t>
+  </si>
+  <si>
+    <t>ISS.011</t>
+  </si>
+  <si>
+    <t>ISS.012</t>
+  </si>
+  <si>
+    <t>ISS.013</t>
+  </si>
+  <si>
+    <t>ISS.014</t>
+  </si>
+  <si>
+    <t>Use of gem 'tzinfo-data' in AWS deployment on Linux servers generates Warning</t>
+  </si>
+  <si>
+    <t>Date Raised</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Mark C</t>
   </si>
 </sst>
 </file>
@@ -343,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -360,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9C0EC-30A0-144D-9AD5-FB8E9C5B121B}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -1097,12 +1161,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E79580C-68E3-4542-A253-6A6ADEE30C34}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="75.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>